<commit_message>
[Feat] REMOVE 패킷 추가
- 접속 해제 시 캐릭터를 지우도록 REMOVE 패킷을 추가함
- remove 메시지 전송 시 방 id가 아닌 플레이어 id로 방 정보를 찾던 버그 수정
</commit_message>
<xml_diff>
--- a/AllInOneGenerator/proto_definitions.xlsx
+++ b/AllInOneGenerator/proto_definitions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Sparta\APOMServer\AllInOneGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980F4421-D600-491E-B356-072BCCC25415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA71A66-2A9B-406E-AB54-7F8EBCED872E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="66">
   <si>
     <t>MessageName</t>
   </si>
@@ -275,6 +275,10 @@
   </si>
   <si>
     <t>L7에서 timeout 체크용. 일정 주기마다 한번씩 서버에 전송</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SC_REMOVE_CHARACTER</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -647,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1087,30 +1091,16 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="B44" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="C44" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D44" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>52</v>
-      </c>
-      <c r="B45" t="s">
-        <v>48</v>
-      </c>
-      <c r="C45" t="s">
-        <v>8</v>
-      </c>
-      <c r="D45" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -1118,13 +1108,13 @@
         <v>52</v>
       </c>
       <c r="B46" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C46" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D46" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -1132,26 +1122,54 @@
         <v>52</v>
       </c>
       <c r="B47" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C47" t="s">
         <v>8</v>
       </c>
       <c r="D47" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>52</v>
+      </c>
+      <c r="B48" t="s">
+        <v>49</v>
+      </c>
+      <c r="C48" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" t="s">
+        <v>59</v>
+      </c>
+      <c r="C49" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>62</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B51" t="s">
         <v>63</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C51" t="s">
         <v>7</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D51" t="s">
         <v>64</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Feat] protoFile 생성기 기능 추가
- enum문 처리 기능 추가
</commit_message>
<xml_diff>
--- a/AllInOneGenerator/proto_definitions.xlsx
+++ b/AllInOneGenerator/proto_definitions.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Sparta\APOMServer\AllInOneGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1E0866-5C05-47BE-9A4E-CB290C749690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBAFFCD4-CC46-429E-B6E8-43F67C82EA7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="645" windowWidth="37035" windowHeight="20355" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Messages" sheetId="1" r:id="rId1"/>
+    <sheet name="AI Scripts" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="77">
   <si>
     <t>MessageName</t>
   </si>
@@ -291,6 +292,37 @@
   </si>
   <si>
     <t>채널 타입, 0번 : 전체, 1번 : 파티, 2번 : 귓속말. 2번일 경우에만 target 검사</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ENUM_BOSS_PHASE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>enum</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDLE</t>
+  </si>
+  <si>
+    <t>ATTACK</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DEATH</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>죽음</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>공격</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>기본</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -663,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -925,18 +957,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" t="s">
-        <v>38</v>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -944,13 +976,13 @@
         <v>37</v>
       </c>
       <c r="B28" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D28" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -958,38 +990,38 @@
         <v>37</v>
       </c>
       <c r="B29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C29" t="s">
         <v>6</v>
       </c>
+      <c r="D29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="B31" t="s">
-        <v>67</v>
+        <v>16</v>
       </c>
       <c r="C31" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D31" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>20</v>
-      </c>
-      <c r="B32" t="s">
-        <v>4</v>
-      </c>
-      <c r="C32" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -997,41 +1029,41 @@
         <v>20</v>
       </c>
       <c r="B33" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="C33" t="s">
         <v>8</v>
       </c>
       <c r="D33" t="s">
-        <v>68</v>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="B35" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C35" t="s">
         <v>8</v>
       </c>
       <c r="D35" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>39</v>
-      </c>
-      <c r="B36" t="s">
-        <v>4</v>
-      </c>
-      <c r="C36" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -1039,41 +1071,41 @@
         <v>39</v>
       </c>
       <c r="B37" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C37" t="s">
         <v>8</v>
       </c>
       <c r="D37" t="s">
-        <v>65</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C39" t="s">
         <v>8</v>
       </c>
       <c r="D39" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>49</v>
-      </c>
-      <c r="B40" t="s">
-        <v>18</v>
-      </c>
-      <c r="C40" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -1081,10 +1113,13 @@
         <v>49</v>
       </c>
       <c r="B41" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C41" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="D41" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -1092,13 +1127,13 @@
         <v>49</v>
       </c>
       <c r="B42" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C42" t="s">
         <v>6</v>
       </c>
       <c r="D42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -1106,55 +1141,52 @@
         <v>49</v>
       </c>
       <c r="B43" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="C43" t="s">
-        <v>51</v>
-      </c>
-      <c r="D43" t="s">
-        <v>53</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44" t="s">
+        <v>16</v>
+      </c>
+      <c r="C44" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="B45" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="C45" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="D45" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="B47" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="C47" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D47" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>51</v>
-      </c>
-      <c r="B48" t="s">
-        <v>47</v>
-      </c>
-      <c r="C48" t="s">
-        <v>8</v>
-      </c>
-      <c r="D48" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -1162,13 +1194,13 @@
         <v>51</v>
       </c>
       <c r="B49" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C49" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D49" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -1176,26 +1208,54 @@
         <v>51</v>
       </c>
       <c r="B50" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C50" t="s">
         <v>8</v>
       </c>
       <c r="D50" t="s">
-        <v>54</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51" t="s">
+        <v>48</v>
+      </c>
+      <c r="C51" t="s">
+        <v>8</v>
+      </c>
+      <c r="D51" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>58</v>
+      </c>
+      <c r="C52" t="s">
+        <v>8</v>
+      </c>
+      <c r="D52" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>61</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B54" t="s">
         <v>62</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C54" t="s">
         <v>7</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D54" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1203,4 +1263,82 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA41E0C3-33FC-4727-B2DD-4CB408971A04}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[Chore] protoFile 생성기 기능 수정
- message 출력 순서 조정. enum, struct, message 순으로 .proto 파일이 만들어지도록 수정
</commit_message>
<xml_diff>
--- a/AllInOneGenerator/proto_definitions.xlsx
+++ b/AllInOneGenerator/proto_definitions.xlsx
@@ -8,20 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Sparta\APOMServer\AllInOneGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBAFFCD4-CC46-429E-B6E8-43F67C82EA7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A724078-1CBA-4BFA-95F4-DC19DD7C8BFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Messages" sheetId="1" r:id="rId1"/>
-    <sheet name="AI Scripts" sheetId="2" r:id="rId2"/>
+    <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Contents" sheetId="3" r:id="rId2"/>
+    <sheet name="AI Scripts" sheetId="2" r:id="rId3"/>
+    <sheet name="Structs" sheetId="6" r:id="rId4"/>
+    <sheet name="Etc" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="98">
   <si>
     <t>MessageName</t>
   </si>
@@ -295,10 +298,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>ENUM_BOSS_PHASE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>enum</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -323,6 +322,87 @@
   </si>
   <si>
     <t>기본</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Position</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>posZ</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>위치</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SC_BOSS_PHASE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>bossID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>보스의 고유 ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOSS_PHASE</t>
+  </si>
+  <si>
+    <t>현재 보스의 페이즈</t>
+  </si>
+  <si>
+    <t xml:space="preserve">currentPhase </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>currentHp</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>보스의 현재 체력</t>
+  </si>
+  <si>
+    <t>maxHp</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>보스의 최대 체력</t>
+  </si>
+  <si>
+    <t>targetPlayerID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>타겟 플레이어의 고유 ID</t>
+  </si>
+  <si>
+    <t>보스가 이동해야 하는 목표 위치</t>
+  </si>
+  <si>
+    <t>targetMovementPos</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>distanceToPlayer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>플레이어와의 현재 거리</t>
+  </si>
+  <si>
+    <t>currentAnimation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>현재 재생되어야하는 애니메이션 정보</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOSS_PHASE</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -695,10 +775,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -862,403 +942,6 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>59</v>
-      </c>
-      <c r="B17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>59</v>
-      </c>
-      <c r="B18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>60</v>
-      </c>
-      <c r="B20" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>60</v>
-      </c>
-      <c r="B21" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>60</v>
-      </c>
-      <c r="B22" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>17</v>
-      </c>
-      <c r="B25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>17</v>
-      </c>
-      <c r="B26" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>37</v>
-      </c>
-      <c r="B28" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>37</v>
-      </c>
-      <c r="B29" t="s">
-        <v>18</v>
-      </c>
-      <c r="C29" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>37</v>
-      </c>
-      <c r="B30" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>37</v>
-      </c>
-      <c r="B31" t="s">
-        <v>16</v>
-      </c>
-      <c r="C31" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>20</v>
-      </c>
-      <c r="B33" t="s">
-        <v>67</v>
-      </c>
-      <c r="C33" t="s">
-        <v>8</v>
-      </c>
-      <c r="D33" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>20</v>
-      </c>
-      <c r="B34" t="s">
-        <v>4</v>
-      </c>
-      <c r="C34" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>20</v>
-      </c>
-      <c r="B35" t="s">
-        <v>21</v>
-      </c>
-      <c r="C35" t="s">
-        <v>8</v>
-      </c>
-      <c r="D35" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>39</v>
-      </c>
-      <c r="B37" t="s">
-        <v>27</v>
-      </c>
-      <c r="C37" t="s">
-        <v>8</v>
-      </c>
-      <c r="D37" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>39</v>
-      </c>
-      <c r="B38" t="s">
-        <v>4</v>
-      </c>
-      <c r="C38" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>39</v>
-      </c>
-      <c r="B39" t="s">
-        <v>21</v>
-      </c>
-      <c r="C39" t="s">
-        <v>8</v>
-      </c>
-      <c r="D39" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>49</v>
-      </c>
-      <c r="B41" t="s">
-        <v>27</v>
-      </c>
-      <c r="C41" t="s">
-        <v>8</v>
-      </c>
-      <c r="D41" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>49</v>
-      </c>
-      <c r="B42" t="s">
-        <v>18</v>
-      </c>
-      <c r="C42" t="s">
-        <v>6</v>
-      </c>
-      <c r="D42" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>49</v>
-      </c>
-      <c r="B43" t="s">
-        <v>19</v>
-      </c>
-      <c r="C43" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>49</v>
-      </c>
-      <c r="B44" t="s">
-        <v>16</v>
-      </c>
-      <c r="C44" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>49</v>
-      </c>
-      <c r="B45" t="s">
-        <v>52</v>
-      </c>
-      <c r="C45" t="s">
-        <v>51</v>
-      </c>
-      <c r="D45" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>64</v>
-      </c>
-      <c r="B47" t="s">
-        <v>27</v>
-      </c>
-      <c r="C47" t="s">
-        <v>8</v>
-      </c>
-      <c r="D47" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>51</v>
-      </c>
-      <c r="B49" t="s">
-        <v>50</v>
-      </c>
-      <c r="C49" t="s">
-        <v>5</v>
-      </c>
-      <c r="D49" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>51</v>
-      </c>
-      <c r="B50" t="s">
-        <v>47</v>
-      </c>
-      <c r="C50" t="s">
-        <v>8</v>
-      </c>
-      <c r="D50" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>51</v>
-      </c>
-      <c r="B51" t="s">
-        <v>48</v>
-      </c>
-      <c r="C51" t="s">
-        <v>8</v>
-      </c>
-      <c r="D51" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>51</v>
-      </c>
-      <c r="B52" t="s">
-        <v>58</v>
-      </c>
-      <c r="C52" t="s">
-        <v>8</v>
-      </c>
-      <c r="D52" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>61</v>
-      </c>
-      <c r="B54" t="s">
-        <v>62</v>
-      </c>
-      <c r="C54" t="s">
-        <v>7</v>
-      </c>
-      <c r="D54" t="s">
-        <v>63</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1266,19 +949,382 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D855BCE1-5701-4923-B770-175E32F8F8C0}">
+  <dimension ref="A1:D32"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="71.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA41E0C3-33FC-4727-B2DD-4CB408971A04}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.875" customWidth="1"/>
+    <col min="3" max="3" width="16.375" customWidth="1"/>
+    <col min="4" max="4" width="35.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -1297,44 +1343,331 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" t="s">
         <v>69</v>
       </c>
-      <c r="B2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C2" t="s">
-        <v>70</v>
-      </c>
       <c r="D2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" t="s">
         <v>69</v>
       </c>
-      <c r="B3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C3" t="s">
-        <v>70</v>
-      </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" t="s">
         <v>69</v>
       </c>
+      <c r="D4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52F83CCD-C06A-4A6A-AE0B-89643DA4CE6B}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>74</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DDB9213-0882-462B-B15C-C1CFF2055437}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Feat] 보스 AI 구성 중
- 기획에 나와 있는대로 구성하는 중
</commit_message>
<xml_diff>
--- a/AllInOneGenerator/proto_definitions.xlsx
+++ b/AllInOneGenerator/proto_definitions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Sparta\APOMServer\AllInOneGenerator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JungSeongUk\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7308F99B-9265-4DA8-9FC0-2FB6937A9902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E9FC3A-1189-4335-9945-33901FF26274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2580" yWindow="600" windowWidth="37035" windowHeight="20355" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="105">
   <si>
     <t>MessageName</t>
   </si>
@@ -302,126 +302,141 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>ATTACK</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Position</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>posZ</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>위치</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SC_BOSS_PHASE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>bossID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>보스의 고유 ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>currentHp</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>보스의 현재 체력</t>
+  </si>
+  <si>
+    <t>maxHp</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>보스의 최대 체력</t>
+  </si>
+  <si>
+    <t>보스가 이동해야 하는 목표 위치</t>
+  </si>
+  <si>
+    <t>targetMovementPos</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>bossPos</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>현재 보스의 위치</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOSS_STATE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>IDLE</t>
-  </si>
-  <si>
-    <t>ATTACK</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>DEATH</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Position</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>posZ</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>위치</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SC_BOSS_PHASE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>bossID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>보스의 고유 ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>BOSS_PHASE</t>
-  </si>
-  <si>
-    <t>현재 보스의 페이즈</t>
-  </si>
-  <si>
-    <t xml:space="preserve">currentPhase </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>currentHp</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>보스의 현재 체력</t>
-  </si>
-  <si>
-    <t>maxHp</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>보스의 최대 체력</t>
-  </si>
-  <si>
-    <t>targetPlayerID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>타겟 플레이어의 고유 ID</t>
-  </si>
-  <si>
-    <t>보스가 이동해야 하는 목표 위치</t>
-  </si>
-  <si>
-    <t>targetMovementPos</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>distanceToPlayer</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>플레이어와의 현재 거리</t>
-  </si>
-  <si>
-    <t>currentAnimation</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>현재 재생되어야하는 애니메이션 정보</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>BOSS_PHASE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>bossPos</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>현재 보스의 위치</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>보스가 사망한 상태</t>
-  </si>
-  <si>
-    <t>광폭화 상태 (체력이 50% 이하일 때)</t>
-  </si>
-  <si>
-    <t>BERSERK</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>RECONFIGURATION</t>
-  </si>
-  <si>
-    <t>패턴 재정비 상태 (체력이 80% 이하일 때)</t>
-  </si>
-  <si>
-    <t>공격 상태 (플레이어에게 접근하거나 공격 중)</t>
-  </si>
-  <si>
-    <t>대기 상태 (그 외의 경우)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>대기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>걷기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>추적</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>공격</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>스킬</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>WALK</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CHASE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>bossState</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>보스의 현재 상태</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKILL3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>스킬1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>스킬2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DIE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>죽음</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>curSpeed</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>현재 이동속도</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1331,10 +1346,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA41E0C3-33FC-4727-B2DD-4CB408971A04}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1361,195 +1376,212 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>103</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D5" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D6" t="s">
-        <v>101</v>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>76</v>
-      </c>
-      <c r="B9" t="s">
-        <v>81</v>
-      </c>
-      <c r="C9" t="s">
-        <v>79</v>
-      </c>
-      <c r="D9" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="B10" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>69</v>
       </c>
       <c r="D10" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="B11" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>69</v>
       </c>
       <c r="D11" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="B12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" t="s">
         <v>89</v>
-      </c>
-      <c r="C12" t="s">
-        <v>73</v>
-      </c>
-      <c r="D12" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="B13" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>69</v>
       </c>
       <c r="D13" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="B14" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>69</v>
       </c>
       <c r="D14" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>85</v>
+      </c>
       <c r="B15" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>69</v>
       </c>
       <c r="D15" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="B16" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C16" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D16" t="s">
-        <v>96</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1646,7 +1678,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
         <v>18</v>
@@ -1655,12 +1687,12 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
@@ -1671,10 +1703,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
[Feat] protoFile 생성기 기능 수정
- repeated 키워드 관련 기능 추가
- 일반 자료형과 구조체를 사용할 경우를 나누어 RPC 코드를 작성
</commit_message>
<xml_diff>
--- a/AllInOneGenerator/proto_definitions.xlsx
+++ b/AllInOneGenerator/proto_definitions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Sparta\APOMServer\AllInOneGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4406EB97-A560-49CB-B1B0-97552AE9BE5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C0FB1F-B650-44F1-8BA2-95296A7FC5A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13470" yWindow="150" windowWidth="37035" windowHeight="20355" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="167">
   <si>
     <t>MessageName</t>
   </si>
@@ -549,14 +549,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>로그인 성공시 해당 캐릭터의 정보를 전송</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SC_TRANSFER_CHARACTER_INFO</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>userName</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -590,6 +582,78 @@
   </si>
   <si>
     <t>CS_FIND_PW_REQUEST</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS_REQUEST_CHARACTER_INFO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS_REQUEST_ITEM_INFO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>bRequest</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>true를 삽입 후 전송할 것</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SC_RESPONSE_CHARACTER_INFO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SC_REQUEST_ITEM_INFO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>클라이언트에서 요청시 해당 캐릭터의 정보를 전송</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>repeated uint32</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>플레이어가 소지하고 있던 아이템 정보</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>itemInfo</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>현재는 아이템의 정보를 uint32 변수 하나로 설정. 나중에 인벤토리의 특정 위치에 있다던가 하는 기능을 넣으면 아이템 구조체를 따로 만들어서 위치까지 저장해 관리해야함</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>서버에게 캐릭터 정보를 요청. 패킷내 모든 변수 값이 0이면 패킷 사이즈가 0이되는 protobuf기 때문에, bool 변수에 true를 줘서 전송해야함</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>서버에게 아이템 정보를 요청. 패킷내 모든 변수 값이 0이면 패킷 사이즈가 0이되는 protobuf기 때문에, bool 변수에 true를 줘서 전송해야함</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>tempData</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SC_TEST_PACKET</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>repeated PlayerInfo</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS_TEST_PACKET1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS_TEST_PACKET2</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -962,19 +1026,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="31.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="68.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="160.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -1058,12 +1122,12 @@
         <v>108</v>
       </c>
       <c r="D7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B9" t="s">
         <v>118</v>
@@ -1111,7 +1175,7 @@
         <v>108</v>
       </c>
       <c r="D13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -1155,10 +1219,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B20" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C20" t="s">
         <v>115</v>
@@ -1197,7 +1261,7 @@
         <v>134</v>
       </c>
       <c r="B24" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C24" t="s">
         <v>115</v>
@@ -1205,19 +1269,103 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="B26" t="s">
+        <v>151</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" t="s">
+        <v>152</v>
+      </c>
+      <c r="E26" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>150</v>
+      </c>
+      <c r="B27" t="s">
+        <v>151</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" t="s">
+        <v>152</v>
+      </c>
+      <c r="E27" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>153</v>
+      </c>
+      <c r="B29" t="s">
         <v>35</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C29" t="s">
         <v>34</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D29" t="s">
         <v>36</v>
       </c>
-      <c r="E26" t="s">
-        <v>140</v>
+      <c r="E29" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>154</v>
+      </c>
+      <c r="B30" t="s">
+        <v>158</v>
+      </c>
+      <c r="C30" t="s">
+        <v>156</v>
+      </c>
+      <c r="D30" t="s">
+        <v>157</v>
+      </c>
+      <c r="E30" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>163</v>
+      </c>
+      <c r="B34" t="s">
+        <v>162</v>
+      </c>
+      <c r="C34" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>165</v>
+      </c>
+      <c r="B35" t="s">
+        <v>162</v>
+      </c>
+      <c r="C35" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>166</v>
+      </c>
+      <c r="B36" t="s">
+        <v>162</v>
+      </c>
+      <c r="C36" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -1231,7 +1379,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1259,16 +1407,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
[Feat] : 패킷 추가
- 파티, AI, 권한 관련
</commit_message>
<xml_diff>
--- a/AllInOneGenerator/proto_definitions.xlsx
+++ b/AllInOneGenerator/proto_definitions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Sparta\APOMServer\AllInOneGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D8204B-2489-46A4-BCAC-7FF521C8A02A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA44162-FB6F-46E2-AD0B-545B8CB972A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="199">
   <si>
     <t>MessageName</t>
   </si>
@@ -221,14 +221,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>SC_BOSS_PHASE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>bossID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>보스의 고유 ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -539,14 +531,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>MaxHP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>몬스터의 최대 HP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>playerJob</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -607,10 +591,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>CS_BOSS_PHASE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>SC_START_AI_CALCULATE</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -631,6 +611,182 @@
   </si>
   <si>
     <t>AI 계산 및 패킷 전송 중단</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>rotateY</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>목표 회전값</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SC_MONSTER_AI</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS_MONSTER_AI</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SC_MONSTER_ROTATE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS_MONSTER_ROTATE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS_CREATE_MONSTER</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SC_PREPARE_ENTERING_DUNGEON</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SC_CANCEL_ENTERING_DUNGEON</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS_REQUEST_ENTER_DUNGEON</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS_CANCEL_ENTERING_DUNGEON</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>던전에 들어가는 것을 취소함. 취소될 시 모든 대기자들에게 취소되었음을 알림</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>bEnter</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>bCancel</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>취소를 누른 플레이어의 id</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>서버쪽에서 방에 들어갈 준비가 되었는지 확인하는 메시지를 대기자들에게 보냄, N초간 대기 후 던전에 접속될 예정. 이 동안 서버에선 방을 만들어 둠.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>던전에 접속 요청을 보냄. 보내는 타이밍은 클라이언트에서 임의로 정함. SC_PREPARE_ENTERING_DUNGEON 패킷 전송 이후 N초 후에 보내면 됨</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS_REQUEST_ENTER_DUNGEON 패킷에 대한 답. 클라이언트는 받을 시 로딩씬으로 넘어감</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SC_RESPONSE_ENTER_DUNGEON_END</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SC_RESPONSE_ENTER_DUNGEON_BEGIN</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS_REQUEST_ENTER_DUNGEON 패킷에 대한 답. 클라이언트는 받을 시 로딩씬이 끝남.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>bEnterBegin</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>bEnterEnd</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>누군가 중간에 취소 버튼을 눌렀으면 버튼을 누른 플레이어의 id를 전송함. 각 클라이언트에선 어떤 플레이어가 취소 버튼을 눌렀다고 알 수 있음.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SC_RESPONSE_ENTER_DUNGEON_END 패킷을 보내기 전까지 다음과 같은 일이 발생함.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS_START_AI_CALCULATE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AI 계산 및 패킷 전송 시작을 서버에 알림</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS_STOP_AI_CALCULATE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AI 계산 및 패킷 전송 중단을 서버에 알림</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS_RESPONSE_ENTER_DUNGEON_END</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>서버에선 SC_START_AI_CALCULATE 패킷을 클라이언트에 전송함. 클라이언트로 부터 답을 받고, 해당 클라이언트가 CS_RESPONSE_ENTER_DUNGEON_END 패킷을 전송하면 이에 대한 패킷을 전송하고 마무리됨</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS_SPAWN_CHARACTER</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>클라이언트에선 이 사이에 몬스터 생성, 플레이어 생성 등을 요청함</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>로딩씬 도중에 더 이상 보낼 패킷이 없다면 전송</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS_MAKE_PARTY</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FromPlayerID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ToPlayerID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SC_MAKE_PARTY</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>파티를 맺는 요청을 보내는 패킷</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>파티를 요청하는 플레이어 ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>파티 요청 대상 플레이어 ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SC_ACCEPT_PARTY</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS_ACCEPT_PARTY</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>파티 요청 수락 패킷</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1005,8 +1161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1034,253 +1190,253 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" t="s">
         <v>83</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E6" t="s">
         <v>84</v>
-      </c>
-      <c r="C6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D6" t="s">
-        <v>100</v>
-      </c>
-      <c r="E6" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E17" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B18" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B20" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C20" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B23" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C23" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E23" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B24" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C24" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B26" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D26" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E26" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B27" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D27" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E27" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B29" t="s">
         <v>33</v>
@@ -1292,24 +1448,24 @@
         <v>34</v>
       </c>
       <c r="E29" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>113</v>
+      </c>
+      <c r="B30" t="s">
+        <v>117</v>
+      </c>
+      <c r="C30" t="s">
         <v>115</v>
       </c>
-      <c r="B30" t="s">
-        <v>119</v>
-      </c>
-      <c r="C30" t="s">
-        <v>117</v>
-      </c>
       <c r="D30" t="s">
+        <v>116</v>
+      </c>
+      <c r="E30" t="s">
         <v>118</v>
-      </c>
-      <c r="E30" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1320,19 +1476,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D855BCE1-5701-4923-B770-175E32F8F8C0}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="71.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="74.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="183.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -1351,16 +1507,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1382,7 +1538,7 @@
         <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C5" t="s">
         <v>46</v>
@@ -1421,7 +1577,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>186</v>
       </c>
       <c r="B9" t="s">
         <v>19</v>
@@ -1433,91 +1589,454 @@
         <v>24</v>
       </c>
     </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>186</v>
+      </c>
+      <c r="B10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+    </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>73</v>
+        <v>186</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>73</v>
+        <v>186</v>
       </c>
       <c r="B12" t="s">
-        <v>135</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>134</v>
-      </c>
-      <c r="E12" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>73</v>
-      </c>
-      <c r="B13" t="s">
-        <v>76</v>
-      </c>
-      <c r="C13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" t="s">
-        <v>77</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>136</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>137</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>161</v>
+      </c>
+      <c r="B16" t="s">
+        <v>133</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>132</v>
+      </c>
+      <c r="E16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>161</v>
+      </c>
+      <c r="B17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" t="s">
+        <v>133</v>
+      </c>
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>132</v>
+      </c>
+      <c r="E20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>149</v>
+      </c>
+      <c r="B23" t="s">
+        <v>152</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>180</v>
+      </c>
+      <c r="B24" t="s">
+        <v>152</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>150</v>
+      </c>
+      <c r="B26" t="s">
+        <v>151</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" t="s">
         <v>154</v>
       </c>
-      <c r="B16" t="s">
-        <v>157</v>
-      </c>
-      <c r="C16" t="s">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>182</v>
+      </c>
+      <c r="B27" t="s">
+        <v>151</v>
+      </c>
+      <c r="C27" t="s">
         <v>7</v>
       </c>
-      <c r="D16" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>155</v>
-      </c>
-      <c r="B17" t="s">
-        <v>156</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="D27" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>189</v>
+      </c>
+      <c r="B29" t="s">
+        <v>190</v>
+      </c>
+      <c r="C29" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" t="s">
+        <v>194</v>
+      </c>
+      <c r="E29" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>189</v>
+      </c>
+      <c r="B30" t="s">
+        <v>191</v>
+      </c>
+      <c r="C30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>192</v>
+      </c>
+      <c r="B32" t="s">
+        <v>190</v>
+      </c>
+      <c r="C32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>192</v>
+      </c>
+      <c r="B33" t="s">
+        <v>191</v>
+      </c>
+      <c r="C33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>197</v>
+      </c>
+      <c r="B35" t="s">
+        <v>190</v>
+      </c>
+      <c r="C35" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" t="s">
+        <v>194</v>
+      </c>
+      <c r="E35" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>197</v>
+      </c>
+      <c r="B36" t="s">
+        <v>191</v>
+      </c>
+      <c r="C36" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>196</v>
+      </c>
+      <c r="B38" t="s">
+        <v>190</v>
+      </c>
+      <c r="C38" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" t="s">
+        <v>194</v>
+      </c>
+      <c r="E38" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>196</v>
+      </c>
+      <c r="B39" t="s">
+        <v>191</v>
+      </c>
+      <c r="C39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>196</v>
+      </c>
+      <c r="B40" t="s">
+        <v>33</v>
+      </c>
+      <c r="C40" t="s">
+        <v>32</v>
+      </c>
+      <c r="D40" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>162</v>
+      </c>
+      <c r="B42" t="s">
+        <v>167</v>
+      </c>
+      <c r="C42" t="s">
         <v>7</v>
       </c>
-      <c r="D17" t="s">
-        <v>159</v>
+      <c r="E42" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>165</v>
+      </c>
+      <c r="B44" t="s">
+        <v>168</v>
+      </c>
+      <c r="C44" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>163</v>
+      </c>
+      <c r="B46" t="s">
+        <v>168</v>
+      </c>
+      <c r="C46" t="s">
+        <v>7</v>
+      </c>
+      <c r="E46" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>163</v>
+      </c>
+      <c r="B47" t="s">
+        <v>19</v>
+      </c>
+      <c r="C47" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>164</v>
+      </c>
+      <c r="B49" t="s">
+        <v>167</v>
+      </c>
+      <c r="C49" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>174</v>
+      </c>
+      <c r="B50" t="s">
+        <v>176</v>
+      </c>
+      <c r="C50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E51" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E52" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E53" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>184</v>
+      </c>
+      <c r="B55" t="s">
+        <v>177</v>
+      </c>
+      <c r="C55" t="s">
+        <v>7</v>
+      </c>
+      <c r="E55" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>173</v>
+      </c>
+      <c r="B56" t="s">
+        <v>177</v>
+      </c>
+      <c r="C56" t="s">
+        <v>7</v>
+      </c>
+      <c r="E56" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -1531,7 +2050,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1650,8 +2169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{511A9449-B0CF-49D2-A97C-3F1A7BDB6056}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1841,182 +2360,182 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>138</v>
+      </c>
+      <c r="B18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" t="s">
         <v>142</v>
-      </c>
-      <c r="B18" t="s">
-        <v>64</v>
-      </c>
-      <c r="C18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" t="s">
-        <v>65</v>
-      </c>
-      <c r="E18" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B19" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
       </c>
       <c r="D19" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B20" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C20" t="s">
         <v>8</v>
       </c>
       <c r="D20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E20" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
       </c>
       <c r="D21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B23" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C23" t="s">
         <v>8</v>
       </c>
       <c r="D23" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E23" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B24" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C24" t="s">
         <v>8</v>
       </c>
       <c r="D24" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B25" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C25" t="s">
         <v>8</v>
       </c>
       <c r="D25" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E25" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" t="s">
         <v>68</v>
-      </c>
-      <c r="C26" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B28" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C28" t="s">
         <v>8</v>
       </c>
       <c r="D28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B29" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C29" t="s">
         <v>8</v>
       </c>
       <c r="D29" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B31" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C31" t="s">
         <v>8</v>
       </c>
       <c r="D31" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B32" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C32" t="s">
         <v>8</v>
       </c>
       <c r="D32" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2027,10 +2546,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA41E0C3-33FC-4727-B2DD-4CB408971A04}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2057,198 +2576,254 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C5" t="s">
         <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C6" t="s">
         <v>46</v>
       </c>
       <c r="D6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>157</v>
+      </c>
+      <c r="B10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
         <v>49</v>
-      </c>
-      <c r="B10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>157</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>157</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>157</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C13" t="s">
         <v>46</v>
       </c>
       <c r="D13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>157</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C14" t="s">
         <v>46</v>
       </c>
       <c r="D14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>157</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>157</v>
       </c>
       <c r="B16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>63</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>159</v>
+      </c>
+      <c r="B18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>159</v>
+      </c>
+      <c r="B19" t="s">
+        <v>155</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>160</v>
+      </c>
+      <c r="B21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>160</v>
+      </c>
+      <c r="B22" t="s">
+        <v>155</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -2262,7 +2837,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2306,13 +2881,13 @@
         <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -2320,13 +2895,13 @@
         <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -2454,44 +3029,44 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" t="s">
         <v>123</v>
       </c>
-      <c r="C2" t="s">
-        <v>125</v>
-      </c>
       <c r="E2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E3" t="s">
         <v>126</v>
-      </c>
-      <c r="B3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C3" t="s">
-        <v>117</v>
-      </c>
-      <c r="E3" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4" t="s">
         <v>123</v>
       </c>
-      <c r="C4" t="s">
-        <v>125</v>
-      </c>
       <c r="E4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Feat] : posSync 패킷 수정
- 기존 x,z 만 보내는 것을 x,y,z 모두 보내는 것으로 수정
</commit_message>
<xml_diff>
--- a/AllInOneGenerator/proto_definitions.xlsx
+++ b/AllInOneGenerator/proto_definitions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Sparta\APOMServer\AllInOneGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1647F8C5-9ACD-433C-95E2-EDC9C5049808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{482AAECE-97E7-4D38-9196-0D752D8E3D45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="202">
   <si>
     <t>MessageName</t>
   </si>
@@ -1492,8 +1492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D855BCE1-5701-4923-B770-175E32F8F8C0}">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2181,10 +2181,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{511A9449-B0CF-49D2-A97C-3F1A7BDB6056}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2310,27 +2310,24 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
       </c>
-      <c r="D11" t="s">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -2338,13 +2335,13 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -2352,10 +2349,13 @@
         <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -2363,49 +2363,40 @@
         <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
       </c>
-      <c r="D16" t="s">
-        <v>29</v>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>136</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>61</v>
-      </c>
-      <c r="E18" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>136</v>
-      </c>
-      <c r="B19" t="s">
-        <v>128</v>
-      </c>
-      <c r="C19" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" t="s">
-        <v>129</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B20" t="s">
         <v>60</v>
@@ -2422,52 +2413,52 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>136</v>
+      </c>
+      <c r="B21" t="s">
+        <v>128</v>
+      </c>
+      <c r="C21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>142</v>
       </c>
-      <c r="B21" t="s">
-        <v>64</v>
-      </c>
-      <c r="C21" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" t="s">
-        <v>65</v>
+      <c r="B22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B23" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C23" t="s">
         <v>8</v>
       </c>
       <c r="D23" t="s">
-        <v>143</v>
-      </c>
-      <c r="E23" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>138</v>
-      </c>
-      <c r="B24" t="s">
-        <v>64</v>
-      </c>
-      <c r="C24" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" t="s">
-        <v>144</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B25" t="s">
         <v>62</v>
@@ -2476,7 +2467,7 @@
         <v>8</v>
       </c>
       <c r="D25" t="s">
-        <v>63</v>
+        <v>143</v>
       </c>
       <c r="E25" t="s">
         <v>139</v>
@@ -2484,7 +2475,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B26" t="s">
         <v>64</v>
@@ -2493,62 +2484,93 @@
         <v>8</v>
       </c>
       <c r="D26" t="s">
-        <v>66</v>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>137</v>
+      </c>
+      <c r="B27" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>137</v>
+      </c>
+      <c r="B28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>145</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B30" t="s">
         <v>62</v>
       </c>
-      <c r="C28" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>67</v>
-      </c>
-      <c r="B29" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="C30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>146</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B33" t="s">
         <v>60</v>
       </c>
-      <c r="C31" t="s">
-        <v>8</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="C33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>141</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B34" t="s">
         <v>60</v>
       </c>
-      <c r="C32" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="C34" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2562,7 +2584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA41E0C3-33FC-4727-B2DD-4CB408971A04}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>

</xml_diff>